<commit_message>
funcionan agunos métodos ya
</commit_message>
<xml_diff>
--- a/xlsx/libro1.xlsx
+++ b/xlsx/libro1.xlsx
@@ -397,15 +397,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Nuevo valor</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="str">
+        <v>nuevaFila</v>
+      </c>
+      <c r="C3" t="str">
+        <v>valor1</v>
+      </c>
+      <c r="D3" t="str">
+        <v>valor2</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>